<commit_message>
Add a bound on 2020 emissions
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_2020_Bounds.xlsx
+++ b/SuppXLS/Scen_SYS_2020_Bounds.xlsx
@@ -8,15 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3D3184-D413-4D64-988D-4C93070A73B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27C1A00-5E1F-472C-83D1-32736E6FD69B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
-    <sheet name="INS" sheetId="2" r:id="rId2"/>
+    <sheet name="TRA_NCAP" sheetId="2" r:id="rId2"/>
     <sheet name="New vehicle sales" sheetId="6" r:id="rId3"/>
+    <sheet name="emi_config" sheetId="17" r:id="rId4"/>
+    <sheet name="emi_single" sheetId="18" r:id="rId5"/>
+    <sheet name="emi_multi" sheetId="19" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
+    <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
+    <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -93,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="264">
   <si>
     <t>Year</t>
   </si>
@@ -858,6 +875,66 @@
   <si>
     <t>*National</t>
   </si>
+  <si>
+    <t>UC_N</t>
+  </si>
+  <si>
+    <t>UC_desc</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>T-A*INT*,T-NAV*</t>
+  </si>
+  <si>
+    <t>Cset_CN</t>
+  </si>
+  <si>
+    <t>*CO2*,-*CO2S</t>
+  </si>
+  <si>
+    <t>Cset_Set</t>
+  </si>
+  <si>
+    <t>ENV</t>
+  </si>
+  <si>
+    <t>Other_indexes</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>UC_FLO</t>
+  </si>
+  <si>
+    <t>UC_COMNET</t>
+  </si>
+  <si>
+    <t>UC - Each Region/All Periods</t>
+  </si>
+  <si>
+    <t>~UC_Sets: T_S:</t>
+  </si>
+  <si>
+    <t>UC_RHSRTS</t>
+  </si>
+  <si>
+    <t>UC_Desc</t>
+  </si>
+  <si>
+    <t>*Units</t>
+  </si>
+  <si>
+    <t>*kt</t>
+  </si>
+  <si>
+    <t>UC - All Regions/Each Period</t>
+  </si>
+  <si>
+    <t>UC_RHSTS</t>
+  </si>
 </sst>
 </file>
 
@@ -869,7 +946,7 @@
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -991,8 +1068,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1050,6 +1134,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFDE9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1408,7 +1504,7 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1488,6 +1584,12 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="273">
     <cellStyle name="20% - Accent5 2" xfId="13" xr:uid="{10C4E126-2686-43C7-AD29-7BC90D313B29}"/>
@@ -1844,6 +1946,114 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Regions"/>
+      <sheetName val="config"/>
+      <sheetName val="single"/>
+      <sheetName val="multi"/>
+      <sheetName val="negative_CO2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>IE</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>National</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>IE-CW</v>
+          </cell>
+          <cell r="F3" t="str">
+            <v>IE-D</v>
+          </cell>
+          <cell r="G3" t="str">
+            <v>IE-KE</v>
+          </cell>
+          <cell r="H3" t="str">
+            <v>IE-KK</v>
+          </cell>
+          <cell r="I3" t="str">
+            <v>IE-LS</v>
+          </cell>
+          <cell r="J3" t="str">
+            <v>IE-LD</v>
+          </cell>
+          <cell r="K3" t="str">
+            <v>IE-LH</v>
+          </cell>
+          <cell r="L3" t="str">
+            <v>IE-MH</v>
+          </cell>
+          <cell r="M3" t="str">
+            <v>IE-OY</v>
+          </cell>
+          <cell r="N3" t="str">
+            <v>IE-WH</v>
+          </cell>
+          <cell r="O3" t="str">
+            <v>IE-WX</v>
+          </cell>
+          <cell r="P3" t="str">
+            <v>IE-WW</v>
+          </cell>
+          <cell r="Q3" t="str">
+            <v>IE-CE</v>
+          </cell>
+          <cell r="R3" t="str">
+            <v>IE-CO</v>
+          </cell>
+          <cell r="S3" t="str">
+            <v>IE-KY</v>
+          </cell>
+          <cell r="T3" t="str">
+            <v>IE-LK</v>
+          </cell>
+          <cell r="U3" t="str">
+            <v>IE-TA</v>
+          </cell>
+          <cell r="V3" t="str">
+            <v>IE-WD</v>
+          </cell>
+          <cell r="W3" t="str">
+            <v>IE-G</v>
+          </cell>
+          <cell r="X3" t="str">
+            <v>IE-LM</v>
+          </cell>
+          <cell r="Y3" t="str">
+            <v>IE-MO</v>
+          </cell>
+          <cell r="Z3" t="str">
+            <v>IE-RN</v>
+          </cell>
+          <cell r="AA3" t="str">
+            <v>IE-SO</v>
+          </cell>
+          <cell r="AB3" t="str">
+            <v>IE-CN</v>
+          </cell>
+          <cell r="AC3" t="str">
+            <v>IE-DL</v>
+          </cell>
+          <cell r="AD3" t="str">
+            <v>IE-MN</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2168,7 +2378,7 @@
   <dimension ref="A3:AD37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2960,7 +3170,7 @@
   <dimension ref="A1:AH24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH9" sqref="AH9"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4423,8 +4633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AC129"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5705,4 +5915,450 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E894F25-B177-4255-B4D5-BD4DFEB7A0BB}">
+  <dimension ref="B4:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="19"/>
+    <col min="2" max="2" width="14" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="9.140625" style="19"/>
+    <col min="11" max="11" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="19" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","Emissions","CO2","2020")</f>
+        <v>UC_Emissions_CO2_2020</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5" s="19" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"CO2 Emissions in 2020")</f>
+        <v>CO2 Emissions in 2020</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="19">
+        <v>2020</v>
+      </c>
+      <c r="D6" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="19">
+        <v>35044</v>
+      </c>
+      <c r="D7" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="19" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="C13" s="19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" s="19">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B54196-8A95-476E-9042-3BA72963A05C}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="19"/>
+    <col min="2" max="2" width="28.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="19"/>
+    <col min="8" max="8" width="12.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="45" t="str">
+        <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,[1]Regions!C3)</f>
+        <v>~UC_Sets: R_E: IE</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="45" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G4" s="19" t="str">
+        <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
+        <v>~UC_T</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="46" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>248</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>255</v>
+      </c>
+      <c r="I5" s="48" t="s">
+        <v>254</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>258</v>
+      </c>
+      <c r="K5" s="46" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20" t="s">
+        <v>261</v>
+      </c>
+      <c r="K6" s="50"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="str">
+        <f>VLOOKUP(B$5, emi_config!$B$4:$D$14,2,FALSE) &amp; "_Single"</f>
+        <v>UC_Emissions_CO2_2020_Single</v>
+      </c>
+      <c r="C7" s="19" t="str">
+        <f>VLOOKUP(C$5, emi_config!$B$4:$D$14,MATCH($F7,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D7" s="19" t="str">
+        <f>VLOOKUP(D$5, emi_config!$B$4:$D$14,MATCH($F7,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F7" s="19">
+        <v>2020</v>
+      </c>
+      <c r="G7" s="19" t="str">
+        <f>VLOOKUP(G$5, emi_config!$B$4:$D$14,MATCH($F7,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H7" s="19">
+        <f>VLOOKUP(H$5, emi_config!$B$4:$D$14,MATCH($F7,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="19">
+        <f>VLOOKUP("Value", emi_config!$B$4:$D$14,MATCH($F7,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>35044</v>
+      </c>
+      <c r="K7" s="19" t="str">
+        <f>VLOOKUP(K$5, emi_config!$B$4:$D$14,2,FALSE) &amp; " - Single"</f>
+        <v>CO2 Emissions in 2020 - Single</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="19" t="str">
+        <f>VLOOKUP(C$5, emi_config!$B$4:$D$14,MATCH($F8,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D8" s="19" t="str">
+        <f>VLOOKUP(D$5, emi_config!$B$4:$D$14,MATCH($F8,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E8" s="19" t="str">
+        <f>VLOOKUP(E$5, emi_config!$B$4:$D$14,MATCH($F8,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F8" s="19">
+        <f>F7</f>
+        <v>2020</v>
+      </c>
+      <c r="I8" s="19">
+        <f>VLOOKUP(I$5, emi_config!$B$4:$D$14,MATCH($F8,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F9" s="19">
+        <v>0</v>
+      </c>
+      <c r="J9" s="19">
+        <f>VLOOKUP("Value", emi_config!$B$4:$D$14,MATCH($F9,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940308C3-5E7F-44AF-A248-ED23EE280DA3}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="19"/>
+    <col min="2" max="2" width="27.28515625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="45" t="str">
+        <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,[1]Regions!D3:AD3)</f>
+        <v>~UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="45" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G4" s="19" t="str">
+        <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
+        <v>~UC_T</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="46" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>248</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>255</v>
+      </c>
+      <c r="I5" s="48" t="s">
+        <v>254</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>263</v>
+      </c>
+      <c r="K5" s="46" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20" t="s">
+        <v>261</v>
+      </c>
+      <c r="K6" s="20"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="str">
+        <f>VLOOKUP(B$5, emi_config!$B$4:$D$14,2,FALSE) &amp; "_Multi"</f>
+        <v>UC_Emissions_CO2_2020_Multi</v>
+      </c>
+      <c r="C7" s="19" t="str">
+        <f>VLOOKUP(C$5, emi_config!$B$4:$D$14,MATCH($F7,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D7" s="19" t="str">
+        <f>VLOOKUP(D$5, emi_config!$B$4:$D$14,MATCH($F7,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="F7" s="19">
+        <v>2020</v>
+      </c>
+      <c r="G7" s="19" t="str">
+        <f>VLOOKUP(G$5, emi_config!$B$4:$D$14,MATCH($F7,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>UP</v>
+      </c>
+      <c r="H7" s="19">
+        <f>VLOOKUP(H$5, emi_config!$B$4:$D$14,MATCH($F7,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="19">
+        <f>VLOOKUP("Value", emi_config!$B$4:$D$14,MATCH($F7,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>35044</v>
+      </c>
+      <c r="K7" s="19" t="str">
+        <f>VLOOKUP(K$5, emi_config!$B$4:$D$14,2,FALSE) &amp; " - Multi"</f>
+        <v>CO2 Emissions in 2020 - Multi</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="19" t="str">
+        <f>VLOOKUP(C$5, emi_config!$B$4:$D$14,MATCH($F8,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+      <c r="D8" s="19" t="str">
+        <f>VLOOKUP(D$5, emi_config!$B$4:$D$14,MATCH($F8,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>ENV</v>
+      </c>
+      <c r="E8" s="19" t="str">
+        <f>VLOOKUP(E$5, emi_config!$B$4:$D$14,MATCH($F8,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>T-A*INT*,T-NAV*</v>
+      </c>
+      <c r="F8" s="19">
+        <f>F7</f>
+        <v>2020</v>
+      </c>
+      <c r="I8" s="19">
+        <f>VLOOKUP(I$5, emi_config!$B$4:$D$14,MATCH($F8,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F9" s="19">
+        <v>0</v>
+      </c>
+      <c r="J9" s="19">
+        <f>VLOOKUP("Value", emi_config!$B$4:$D$14,MATCH($F9,emi_config!$B$6:$D$6,),FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>